<commit_message>
stat done, before flipping location
</commit_message>
<xml_diff>
--- a/Assets/Studies/CHI26_Study1_Funneling/data_processing/analysis/p16/p16_analysis.xlsx
+++ b/Assets/Studies/CHI26_Study1_Funneling/data_processing/analysis/p16/p16_analysis.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4352,6 +4352,9 @@
       <c r="A137">
         <v>16</v>
       </c>
+      <c r="B137">
+        <v>141</v>
+      </c>
       <c r="C137">
         <v>9</v>
       </c>
@@ -4361,8 +4364,17 @@
       <c r="E137">
         <v>0.5</v>
       </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
       <c r="H137">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>-0.5</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4370,28 +4382,28 @@
         <v>16</v>
       </c>
       <c r="B138">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C138">
-        <v>9</v>
+        <v>-15</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G138">
-        <v>0</v>
+        <v>0.7968627</v>
       </c>
       <c r="H138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I138">
-        <v>1</v>
+        <v>-0.2968627</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4399,28 +4411,28 @@
         <v>16</v>
       </c>
       <c r="B139">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C139">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H139">
         <v>1</v>
       </c>
       <c r="I139">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4428,13 +4440,13 @@
         <v>16</v>
       </c>
       <c r="B140">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C140">
-        <v>-15</v>
+        <v>9</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -4443,13 +4455,13 @@
         <v>1</v>
       </c>
       <c r="G140">
-        <v>0.1950042</v>
+        <v>1</v>
       </c>
       <c r="H140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I140">
-        <v>0.8049958</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4457,28 +4469,28 @@
         <v>16</v>
       </c>
       <c r="B141">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C141">
-        <v>-15</v>
+        <v>9</v>
       </c>
       <c r="D141">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E141">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>0.1950042</v>
       </c>
       <c r="H141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I141">
-        <v>0.5</v>
+        <v>-0.1950042</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4486,28 +4498,28 @@
         <v>16</v>
       </c>
       <c r="B142">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C142">
-        <v>9</v>
+        <v>-15</v>
       </c>
       <c r="D142">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E142">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F142">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G142">
-        <v>0.2539699</v>
+        <v>0.9218271</v>
       </c>
       <c r="H142">
         <v>1</v>
       </c>
       <c r="I142">
-        <v>0.2460301</v>
+        <v>0.07817289999999999</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -4515,10 +4527,10 @@
         <v>16</v>
       </c>
       <c r="B143">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C143">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -4527,16 +4539,16 @@
         <v>1</v>
       </c>
       <c r="F143">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G143">
-        <v>0.2966696</v>
+        <v>1</v>
       </c>
       <c r="H143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I143">
-        <v>0.7033304</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4544,28 +4556,28 @@
         <v>16</v>
       </c>
       <c r="B144">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="E144">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F144">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G144">
-        <v>0.2275373</v>
+        <v>1</v>
       </c>
       <c r="H144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I144">
-        <v>0.5224626999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4573,28 +4585,28 @@
         <v>16</v>
       </c>
       <c r="B145">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="D145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E145">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F145">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G145">
-        <v>0.2255039</v>
+        <v>0.6484309</v>
       </c>
       <c r="H145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I145">
-        <v>0.5244961</v>
+        <v>-0.1484309</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -4602,28 +4614,28 @@
         <v>16</v>
       </c>
       <c r="B146">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D146">
         <v>1</v>
       </c>
       <c r="E146">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G146">
-        <v>0.7378967</v>
+        <v>0.2702366</v>
       </c>
       <c r="H146">
         <v>1</v>
       </c>
       <c r="I146">
-        <v>0.01210330000000004</v>
+        <v>-0.02023659999999999</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -4631,10 +4643,10 @@
         <v>16</v>
       </c>
       <c r="B147">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="D147">
         <v>0.1</v>
@@ -4643,16 +4655,16 @@
         <v>0</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G147">
-        <v>1</v>
+        <v>0.1685711</v>
       </c>
       <c r="H147">
         <v>1</v>
       </c>
       <c r="I147">
-        <v>-1</v>
+        <v>-0.1685711</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -4660,28 +4672,28 @@
         <v>16</v>
       </c>
       <c r="B148">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D148">
         <v>2</v>
       </c>
       <c r="E148">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="F148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G148">
-        <v>1</v>
+        <v>0.2539699</v>
       </c>
       <c r="H148">
         <v>1</v>
       </c>
       <c r="I148">
-        <v>0</v>
+        <v>-0.003969900000000026</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -4689,28 +4701,28 @@
         <v>16</v>
       </c>
       <c r="B149">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="C149">
-        <v>-15</v>
+        <v>9</v>
       </c>
       <c r="D149">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E149">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F149">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G149">
-        <v>1</v>
+        <v>0.8578616999999999</v>
       </c>
       <c r="H149">
         <v>1</v>
       </c>
       <c r="I149">
-        <v>-0.75</v>
+        <v>-0.3578616999999999</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -4718,28 +4730,28 @@
         <v>16</v>
       </c>
       <c r="B150">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="C150">
         <v>-15</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E150">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F150">
         <v>-1</v>
       </c>
       <c r="G150">
-        <v>0.2223705</v>
+        <v>0.2966696</v>
       </c>
       <c r="H150">
         <v>1</v>
       </c>
       <c r="I150">
-        <v>0.2776295</v>
+        <v>-0.04666959999999998</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -4747,16 +4759,695 @@
         <v>16</v>
       </c>
       <c r="B151">
+        <v>156</v>
+      </c>
+      <c r="C151">
+        <v>9</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+      <c r="G151">
+        <v>0.8842947</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="I151">
+        <v>0.1157053</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152">
+        <v>16</v>
+      </c>
+      <c r="B152">
+        <v>157</v>
+      </c>
+      <c r="C152">
+        <v>-15</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>-1</v>
+      </c>
+      <c r="G152">
+        <v>0.2275373</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="I152">
+        <v>-0.2275373</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="A153">
+        <v>16</v>
+      </c>
+      <c r="B153">
+        <v>158</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>2</v>
+      </c>
+      <c r="E153">
+        <v>0.75</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="I153">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154">
+        <v>16</v>
+      </c>
+      <c r="B154">
+        <v>160</v>
+      </c>
+      <c r="C154">
+        <v>9</v>
+      </c>
+      <c r="D154">
+        <v>0.1</v>
+      </c>
+      <c r="E154">
+        <v>0.5</v>
+      </c>
+      <c r="F154">
+        <v>1</v>
+      </c>
+      <c r="G154">
+        <v>0.5894653</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+      <c r="I154">
+        <v>-0.08946529999999997</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155">
+        <v>16</v>
+      </c>
+      <c r="B155">
+        <v>161</v>
+      </c>
+      <c r="C155">
+        <v>-15</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <v>-1</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+      <c r="H155">
+        <v>1</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156">
+        <v>16</v>
+      </c>
+      <c r="B156">
+        <v>162</v>
+      </c>
+      <c r="C156">
+        <v>9</v>
+      </c>
+      <c r="D156">
+        <v>2</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="G156">
+        <v>0.2255039</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+      <c r="I156">
+        <v>-0.2255039</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157">
+        <v>16</v>
+      </c>
+      <c r="B157">
+        <v>163</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>2</v>
+      </c>
+      <c r="E157">
+        <v>0.75</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>0.9452937</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="I157">
+        <v>-0.1952937</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158">
+        <v>16</v>
+      </c>
+      <c r="B158">
+        <v>164</v>
+      </c>
+      <c r="C158">
+        <v>9</v>
+      </c>
+      <c r="D158">
+        <v>0.1</v>
+      </c>
+      <c r="E158">
+        <v>0.75</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+      <c r="G158">
+        <v>0.9615609000000001</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="I158">
+        <v>-0.2115609000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159">
+        <v>16</v>
+      </c>
+      <c r="B159">
+        <v>165</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
+      <c r="E159">
+        <v>0.5</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>0.6972303</v>
+      </c>
+      <c r="H159">
+        <v>1</v>
+      </c>
+      <c r="I159">
+        <v>-0.1972303</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="A160">
+        <v>16</v>
+      </c>
+      <c r="B160">
+        <v>166</v>
+      </c>
+      <c r="C160">
+        <v>9</v>
+      </c>
+      <c r="D160">
+        <v>2</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>1</v>
+      </c>
+      <c r="G160">
+        <v>0.319036</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+      <c r="I160">
+        <v>-0.319036</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
+      <c r="A161">
+        <v>16</v>
+      </c>
+      <c r="B161">
+        <v>167</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>0.5</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="G161">
+        <v>0.7378967</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+      <c r="I161">
+        <v>-0.2378967</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162">
+        <v>16</v>
+      </c>
+      <c r="B162">
+        <v>168</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>0.75</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="I162">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163">
+        <v>16</v>
+      </c>
+      <c r="B163">
+        <v>169</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0.1</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="G163">
+        <v>0.2051709</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
+      <c r="I163">
+        <v>-0.2051709</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164">
+        <v>16</v>
+      </c>
+      <c r="B164">
+        <v>170</v>
+      </c>
+      <c r="C164">
+        <v>9</v>
+      </c>
+      <c r="D164">
+        <v>2</v>
+      </c>
+      <c r="E164">
+        <v>0.5</v>
+      </c>
+      <c r="F164">
+        <v>1</v>
+      </c>
+      <c r="G164">
+        <v>0.9676601</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="I164">
+        <v>-0.4676601</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165">
+        <v>16</v>
+      </c>
+      <c r="B165">
+        <v>171</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165">
+        <v>0.75</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <v>1</v>
+      </c>
+      <c r="H165">
+        <v>1</v>
+      </c>
+      <c r="I165">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166">
+        <v>16</v>
+      </c>
+      <c r="B166">
+        <v>172</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166">
+        <v>2</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166">
+        <v>0.9778268</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+      <c r="I166">
+        <v>0.0221732</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167">
+        <v>16</v>
+      </c>
+      <c r="B167">
+        <v>173</v>
+      </c>
+      <c r="C167">
+        <v>-15</v>
+      </c>
+      <c r="D167">
+        <v>0.1</v>
+      </c>
+      <c r="E167">
+        <v>0.5</v>
+      </c>
+      <c r="F167">
+        <v>-1</v>
+      </c>
+      <c r="G167">
+        <v>0.8273624000000001</v>
+      </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
+      <c r="I167">
+        <v>-0.3273624000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168">
+        <v>16</v>
+      </c>
+      <c r="B168">
+        <v>174</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>0.25</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <v>0.2011043</v>
+      </c>
+      <c r="H168">
+        <v>1</v>
+      </c>
+      <c r="I168">
+        <v>0.04889569999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169">
+        <v>16</v>
+      </c>
+      <c r="B169">
+        <v>175</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>0.1</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="G169">
+        <v>0.9269941</v>
+      </c>
+      <c r="H169">
+        <v>1</v>
+      </c>
+      <c r="I169">
+        <v>0.07300589999999996</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170">
+        <v>16</v>
+      </c>
+      <c r="B170">
+        <v>176</v>
+      </c>
+      <c r="C170">
+        <v>9</v>
+      </c>
+      <c r="D170">
+        <v>2</v>
+      </c>
+      <c r="E170">
+        <v>0.75</v>
+      </c>
+      <c r="F170">
+        <v>1</v>
+      </c>
+      <c r="G170">
+        <v>1</v>
+      </c>
+      <c r="H170">
+        <v>1</v>
+      </c>
+      <c r="I170">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171">
+        <v>16</v>
+      </c>
+      <c r="B171">
+        <v>177</v>
+      </c>
+      <c r="C171">
+        <v>-15</v>
+      </c>
+      <c r="D171">
+        <v>0.1</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>-1</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+      <c r="I171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172">
+        <v>16</v>
+      </c>
+      <c r="B172">
+        <v>178</v>
+      </c>
+      <c r="C172">
+        <v>-15</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>0.25</v>
+      </c>
+      <c r="F172">
+        <v>-1</v>
+      </c>
+      <c r="G172">
+        <v>0.2223705</v>
+      </c>
+      <c r="H172">
+        <v>1</v>
+      </c>
+      <c r="I172">
+        <v>0.0276295</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173">
+        <v>16</v>
+      </c>
+      <c r="B173">
+        <v>179</v>
+      </c>
+      <c r="C173">
+        <v>-15</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+      <c r="E173">
+        <v>0.5</v>
+      </c>
+      <c r="F173">
+        <v>-1</v>
+      </c>
+      <c r="G173">
+        <v>0.2438036</v>
+      </c>
+      <c r="H173">
+        <v>1</v>
+      </c>
+      <c r="I173">
+        <v>0.2561964</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174">
+        <v>16</v>
+      </c>
+      <c r="B174">
         <v>180</v>
       </c>
-      <c r="F151">
-        <v>0</v>
-      </c>
-      <c r="G151">
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>0.1</v>
+      </c>
+      <c r="E174">
+        <v>0.5</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="G174">
         <v>0.5243997</v>
       </c>
-      <c r="H151">
-        <v>0</v>
+      <c r="H174">
+        <v>1</v>
+      </c>
+      <c r="I174">
+        <v>-0.02439970000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>